<commit_message>
Fixed all current table create, constraints and insert bugs
</commit_message>
<xml_diff>
--- a/TODO List.xlsx
+++ b/TODO List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\GitAttempt\Cache-Crusaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E226AD9-9551-4148-9FCB-417E59B7B8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44069192-375A-4763-86CD-CA3E626E6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Cache Crusaders</t>
   </si>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,11 +175,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -216,18 +211,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -292,7 +286,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,11 +385,10 @@
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525" cap="flat" cmpd="sng">
+                <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
                   <a:tailEnd/>
@@ -414,15 +407,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>179784</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>27384</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -432,7 +425,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5005F878-DEEE-2DCF-292A-9561B2684F73}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -481,15 +474,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>178593</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>26193</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -499,7 +492,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EFE3DB-76A1-A8E2-191C-AC6E39090E8B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -548,15 +541,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>177402</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>25002</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -566,7 +559,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A790CACC-B062-E3BD-B5F3-17DC7632350A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -615,15 +608,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>176211</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>23811</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -633,7 +626,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27306655-36B2-0CF6-7846-7889FEDE155D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -682,15 +675,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>175020</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>22620</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -700,7 +693,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB058A2D-CDF2-6100-857A-825051F96DF0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -749,15 +742,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>173829</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>21429</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -767,7 +760,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C857E102-BDC5-147F-3F48-0B5A15B7BD18}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -816,15 +809,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>172638</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>20238</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -834,7 +827,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE6C00A-9AE5-AE0E-6F10-D8230B4947F6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -883,13 +876,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>338137</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -901,7 +894,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB098F82-FC11-1622-31EC-66EB8B2B1DD0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -947,14 +940,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109538</xdr:colOff>
+          <xdr:colOff>114300</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228599" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -963,7 +961,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A401A62-4264-4AC1-A652-1001B3219785}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1003,20 +1001,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>179784</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
@@ -1025,7 +1028,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F3764E-9D3C-4F0C-AF83-CD67F2049C36}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1065,20 +1068,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>178593</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -1087,7 +1095,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D378A0DF-D593-47CE-9573-7BE15052E5AB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1127,20 +1135,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>177402</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -1149,7 +1162,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DA2DF8-3A65-407B-9B01-6021DB480F3D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1189,20 +1202,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>176211</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -1211,7 +1229,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7837A06-FAEB-4A1F-86D6-FAB97B2C2641}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1251,20 +1269,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>175020</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -1273,7 +1296,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C07B7E6-D10D-4856-B8DD-7E238E767B89}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1313,20 +1336,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>173829</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1335,7 +1363,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5874DCE2-CBFF-4777-BA93-4AAB8B639B92}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1375,20 +1403,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>172638</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1397,7 +1430,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02EF84C1-F577-4BBE-A756-2B3652B6F3D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1437,20 +1470,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>176211</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -1459,7 +1497,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FD6C6A1-2ECD-4C46-B8FF-DCE3C8D2E057}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1499,20 +1537,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>175020</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -1521,7 +1564,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77420D87-9DD4-4CA4-88A6-9731BD2437F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1561,20 +1604,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>173829</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
@@ -1583,7 +1631,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FB8FD96-738A-43D1-B46C-5DDFCE6333A5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1623,20 +1671,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>172638</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
@@ -1645,7 +1698,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF4CEF5F-6B1A-4DF8-B7C8-934B70B33205}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1685,20 +1738,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>109537</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -1707,7 +1765,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89044298-35D8-4C8A-9C8D-11F629697EED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1747,7 +1805,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1764,7 +1822,7 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>333375</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1774,7 +1832,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9917256-67D7-777D-5205-7381D40E5322}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2139,10 +2197,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDE03D1-9076-45E4-B59F-B85AFA43941D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,60 +2218,60 @@
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2230,7 +2288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2240,11 +2298,14 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2258,7 +2319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>14</v>
       </c>
@@ -2266,7 +2327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>15</v>
       </c>
@@ -2274,7 +2335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -2282,7 +2343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>17</v>
       </c>
@@ -2290,7 +2351,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>18</v>
       </c>
@@ -2298,31 +2359,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finished constraints and cleaned up files
</commit_message>
<xml_diff>
--- a/TODO List.xlsx
+++ b/TODO List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\GitAttempt\Cache-Crusaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44069192-375A-4763-86CD-CA3E626E6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E719C00-B006-43B0-A574-52FBB10EF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
+    <workbookView xWindow="3990" yWindow="2970" windowWidth="19620" windowHeight="11295" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,11 +306,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2200,7 +2200,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Slight added to todo list
</commit_message>
<xml_diff>
--- a/TODO List.xlsx
+++ b/TODO List.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\GitAttempt\Cache-Crusaders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\CacheCrusaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E719C00-B006-43B0-A574-52FBB10EF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA126940-0D95-48CF-B582-BCA32003B620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2970" windowWidth="19620" windowHeight="11295" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main Stuff" sheetId="1" r:id="rId1"/>
+    <sheet name="Queries" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Cache Crusaders</t>
   </si>
@@ -138,6 +139,24 @@
   </si>
   <si>
     <t>Fanie</t>
+  </si>
+  <si>
+    <t>Jaundre/Franco</t>
+  </si>
+  <si>
+    <t>Fanie/Jaundre</t>
+  </si>
+  <si>
+    <t>Renier</t>
+  </si>
+  <si>
+    <t>Sequences</t>
+  </si>
+  <si>
+    <t>Franco</t>
+  </si>
+  <si>
+    <t>Database Queries</t>
   </si>
 </sst>
 </file>
@@ -228,7 +247,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -305,6 +332,30 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
@@ -314,7 +365,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,7 +381,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1877,6 +1928,400 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0117CC-0560-7FA7-6250-FED255323C5E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA867926-2808-4F43-8D87-27A8F2DD9629}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BADFAA59-A27A-483B-A713-CEE924222AB1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB721201-9F41-447A-B16B-747006AA6866}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F0F0F7-F919-4B53-8558-E4CF15920599}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="228600" cy="228600"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{475D791C-A869-48FB-8230-57979B9C2EB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42BDD176-D073-45F4-96E9-6EAE63FA5625}" name="tblQueries" displayName="tblQueries" ref="A3:C9" totalsRowShown="0">
+  <autoFilter ref="A3:C9" xr:uid="{42BDD176-D073-45F4-96E9-6EAE63FA5625}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A6D62A65-622B-4EA5-ADFC-4C01E5980BD7}" name="Status"/>
+    <tableColumn id="2" xr3:uid="{7AFAD400-D36A-4C47-ADCD-9877C041DDCD}" name="Task"/>
+    <tableColumn id="3" xr3:uid="{A9B400C5-1ADA-471D-8A9A-4AED007D12CC}" name="Completed By"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2199,8 +2644,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2654,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" customWidth="1"/>
@@ -2315,6 +2760,9 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
       <c r="I6" t="s">
         <v>23</v>
       </c>
@@ -2323,6 +2771,9 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" t="s">
         <v>24</v>
       </c>
@@ -2331,6 +2782,9 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
       <c r="I8" t="s">
         <v>25</v>
       </c>
@@ -2339,6 +2793,9 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
       <c r="I9" t="s">
         <v>28</v>
       </c>
@@ -2347,6 +2804,9 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" t="s">
         <v>29</v>
       </c>
@@ -2355,11 +2815,20 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
       <c r="I11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" t="s">
         <v>26</v>
       </c>
@@ -2899,4 +3368,201 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6218E091-96A0-4BA7-916A-2CF021229992}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A4:C9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A4=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2050" r:id="rId3" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId4" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2052" r:id="rId5" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2053" r:id="rId6" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId7" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2055" r:id="rId8" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <tableParts count="1">
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Almal: Completed Database Objects section
</commit_message>
<xml_diff>
--- a/TODO List.xlsx
+++ b/TODO List.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\CacheCrusaders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA126940-0D95-48CF-B582-BCA32003B620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47243869-778C-420B-8879-FACDF258F679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Stuff" sheetId="1" r:id="rId1"/>
-    <sheet name="Queries" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Cache Crusaders</t>
   </si>
@@ -154,9 +153,6 @@
   </si>
   <si>
     <t>Franco</t>
-  </si>
-  <si>
-    <t>Database Queries</t>
   </si>
 </sst>
 </file>
@@ -247,15 +243,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -332,30 +320,6 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
@@ -369,7 +333,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,7 +341,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1928,400 +1892,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0117CC-0560-7FA7-6250-FED255323C5E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA867926-2808-4F43-8D87-27A8F2DD9629}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2052"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BADFAA59-A27A-483B-A713-CEE924222AB1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2053"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB721201-9F41-447A-B16B-747006AA6866}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2054"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F0F0F7-F919-4B53-8558-E4CF15920599}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="228600" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2055"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{475D791C-A869-48FB-8230-57979B9C2EB2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42BDD176-D073-45F4-96E9-6EAE63FA5625}" name="tblQueries" displayName="tblQueries" ref="A3:C9" totalsRowShown="0">
-  <autoFilter ref="A3:C9" xr:uid="{42BDD176-D073-45F4-96E9-6EAE63FA5625}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A6D62A65-622B-4EA5-ADFC-4C01E5980BD7}" name="Status"/>
-    <tableColumn id="2" xr3:uid="{7AFAD400-D36A-4C47-ADCD-9877C041DDCD}" name="Task"/>
-    <tableColumn id="3" xr3:uid="{A9B400C5-1ADA-471D-8A9A-4AED007D12CC}" name="Completed By"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2644,8 +2214,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,201 +2938,4 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6218E091-96A0-4BA7-916A-2CF021229992}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A4:C9">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A4=TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId3" name="Check Box 2">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId4" name="Check Box 3">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2052" r:id="rId5" name="Check Box 4">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2053" r:id="rId6" name="Check Box 5">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId7" name="Check Box 6">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2055" r:id="rId8" name="Check Box 7">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <tableParts count="1">
-    <tablePart r:id="rId9"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added much more example data and completed Queries 4 and 5
</commit_message>
<xml_diff>
--- a/TODO List.xlsx
+++ b/TODO List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaund\Downloads\cc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B518378A-1D79-467B-B0B3-E667B6160AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5147F26-C282-4C18-A25F-778B2D39B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DA4635F5-24E9-4E0A-8B32-3E992EB102DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Stuff" sheetId="1" r:id="rId1"/>
@@ -177,12 +177,6 @@
     <t>Customer_ORDER_Management</t>
   </si>
   <si>
-    <t>PARTS Inventory Check</t>
-  </si>
-  <si>
-    <t>SORTING</t>
-  </si>
-  <si>
     <t>Check_Available_Technicians</t>
   </si>
   <si>
@@ -226,6 +220,12 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Parts Statistics</t>
+  </si>
+  <si>
+    <t>Aggregate functions</t>
   </si>
 </sst>
 </file>
@@ -319,9 +319,6 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -338,6 +335,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -997,7 +997,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{021DD532-B075-4352-B783-F966E736DE73}" name="Table2" displayName="Table2" ref="A3:D19" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{021DD532-B075-4352-B783-F966E736DE73}" name="Table2" displayName="Table2" ref="A3:D19" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:D19" xr:uid="{021DD532-B075-4352-B783-F966E736DE73}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3A36696-C3F4-4B6C-8258-06756F64E2BA}" name="Queries"/>
@@ -1014,7 +1014,7 @@
   <autoFilter ref="G2:H13" xr:uid="{219BE757-8C54-4268-8B9B-FFC45D3EB93A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{76A635AC-7FFE-47DF-867F-0B4F99CF09B2}" name="Requirement"/>
-    <tableColumn id="2" xr3:uid="{0428692A-89B0-4757-B45F-8174ECA6F1BE}" name="Count" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0428692A-89B0-4757-B45F-8174ECA6F1BE}" name="Count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,10 +1737,10 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
@@ -1838,13 +1838,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
         <v>28</v>
@@ -1856,7 +1856,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1871,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -1886,7 +1886,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1901,7 +1901,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1916,7 +1916,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1931,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1942,7 +1942,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1953,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>36</v>
@@ -1964,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -1975,7 +1975,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
@@ -1986,7 +1986,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>

</xml_diff>